<commit_message>
adicioando atualizaçao automatica das estatisticas
</commit_message>
<xml_diff>
--- a/BancoProd.xlsx
+++ b/BancoProd.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C89"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,17 +453,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Número inválido</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>+55 00 00000069</t>
+          <t>+55 69 36421238</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>JOAO BATISTA DE SOUZA - nan - BR 429, KM 1, LT 6, GB 12, STR BR 429 SENT/ALV, CHACAR FUNDIARIA</t>
+          <t>CLAUDIO DA SILVA - SITIO DUAS IRMAS - LH 78 SUL, KM 18, LT 130-A, GB 05, STR BR 429 SENT/SERING || EDIVALDO CARLOS DE OLIVEIRA - ST. FLOR DA MATA - LH 78 SUL, KM 20, LT 144, GB 05, STR BR 429 SENT/SERING || CLAUDIO DA SILVA - SITIO DUAS IRMAS - LH 78 SUL, KM 18, LT 130-A, GB 05, STR BR 429 SENT/SERING || CLAUDIO DA SILVA - SITIO DUAS IRMAS - LH 78 SUL, KM 18, LT 130-A, GB 05, STR BR 429 SENT/SERING</t>
         </is>
       </c>
     </row>
@@ -475,12 +475,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>+55 69 36421238</t>
+          <t>+55 69 984266737</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CLAUDIO DA SILVA - SITIO DUAS IRMAS - LH 78 SUL, KM 18, LT 130-A, GB 05, STR BR 429 SENT/SERING || EDIVALDO CARLOS DE OLIVEIRA - ST. FLOR DA MATA - LH 78 SUL, KM 20, LT 144, GB 05, STR BR 429 SENT/SERING || CLAUDIO DA SILVA - SITIO DUAS IRMAS - LH 78 SUL, KM 18, LT 130-A, GB 05, STR BR 429 SENT/SERING || CLAUDIO DA SILVA - SITIO DUAS IRMAS - LH 78 SUL, KM 18, LT 130-A, GB 05, STR BR 429 SENT/SERING</t>
+          <t>JORGE ALVES RODRIGUES - CHACARA BANDEIRA BRANCA - LH 82 SUL, KM 8, LT 56, GB 4, STR RO 481, DEMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -492,12 +492,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>+55 69 981256679</t>
+          <t>+55 69 984313304</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>EDUARDO DOS SANTOS PENSO - SITIO SAO MIGUEL - LH 09 SUL, KM 10, LT 73, GB 01, STR BR 429 SENT/SERING, DESMEMBRADO</t>
+          <t>ROSA GRAZIELE OLIVEIRA SOUZA CRAUSE - SITIO CATARINA - LH 98 NORTE, KM 11,5, LT 38-B1, GB 16, STR RO 481, TRAVESSAO DA 94 PARA 98 || ROSA GRAZIELE OLIVEIRA SOUZA CRAUSE - SITIO BOM SUCESSO - LH 94 NORTE, KM 4, LT 15, GB 08, STR RO 481, L.E</t>
         </is>
       </c>
     </row>
@@ -509,12 +509,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>+55 69 984266737</t>
+          <t>+55 69 984397155</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>JORGE ALVES RODRIGUES - CHACARA BANDEIRA BRANCA - LH 82 SUL, KM 8, LT 56, GB 4, STR RO 481, DEMEMBRADO</t>
+          <t>LUCIA PEREIRA DOS SANTOS - SITIO TERRA ROXA - ROD. RO 481, KM 17, LT 3, GB RIO BRANCO, STR RO 481, DESMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -526,12 +526,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>+55 69 984313304</t>
+          <t>+55 69 984449468</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ROSA GRAZIELE OLIVEIRA SOUZA CRAUSE - SITIO CATARINA - LH 98 NORTE, KM 11,5, LT 38-B1, GB 16, STR RO 481, TRAVESSAO DA 94 PARA 98 || ROSA GRAZIELE OLIVEIRA SOUZA CRAUSE - SITIO BOM SUCESSO - LH 94 NORTE, KM 4, LT 15, GB 08, STR RO 481, L.E</t>
+          <t>DINALVA SILVA DOS SANTOS - SITIO DOS ANJOS - BR 429, KM 1,5, LT 24, GB 11, STR BR 429 SENT/SERING || DINALVA SILVA DOS SANTOS - CHACARA BOA SORTE - LH 25 (MORTA), KM 6, LT 08, GB 5, STR RO 481 || JAIR SILVA GOMES - CHACARA BOA SORTE - LH 25 (MORTA), KM 6, LT 08, GB 5, STR RO 481 || DINALVA SILVA DOS SANTOS - SITIO DOS ANJOS - BR 429, KM 1,5, LT 24, GB 11, STR BR 429 SENT/SERING || DINALVA SILVA DOS SANTOS - CHACARA BOA SORTE - LH 25 (MORTA), KM 6, LT 08, GB 5, STR RO 481 || DINALVA SILVA DOS SANTOS - SITIO DOS ANJOS - BR 429, KM 1,5, LT 24, GB 11, STR BR 429 SENT/SERING || DINALVA SILVA DOS SANTOS - CHACARA BOA SORTE - LH 25 (MORTA), KM 6, LT 08, GB 5, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -543,12 +543,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>+55 69 984382158</t>
+          <t>+55 69 984521725</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>VANESSA FREIRE DA SILVA - RANCHO VF - LH 86 NORTE, KM 4, LT 33, GB RIO BRANCO, STR BR 429 SENT/ALV</t>
+          <t>CAMILA CAROLINA FERREIRA CRUZ CHOQUE - RANCHO BRASIL - LH 82 NORTE, KM 1, LT 15E, GB 13, STR CHACAREIRO</t>
         </is>
       </c>
     </row>
@@ -560,12 +560,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>+55 69 984397155</t>
+          <t>+55 69 984528653</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>LUCIA PEREIRA DOS SANTOS - SITIO TERRA ROXA - ROD. RO 481, KM 17, LT 3, GB RIO BRANCO, STR RO 481, DESMEMBRADO</t>
+          <t>VANDERLEI DE OLIVEIRA CORDEIRO - SITIO SOLO RICO - LH 86 SUL, KM 20, LT 01B, GB 01, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -577,12 +577,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>+55 69 984449468</t>
+          <t>+55 69 984680406</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>DINALVA SILVA DOS SANTOS - CHACARA BOA SORTE - LH 25 (MORTA), KM 6, LT 08, GB 5, STR RO 481 || DINALVA SILVA DOS SANTOS - SITIO DOS ANJOS - BR 429, KM 1,5, LT 24, GB 11, STR BR 429 SENT/SERING || JAIR SILVA GOMES - CHACARA BOA SORTE - LH 25 (MORTA), KM 6, LT 08, GB 5, STR RO 481 || DINALVA SILVA DOS SANTOS - CHACARA BOA SORTE - LH 25 (MORTA), KM 6, LT 08, GB 5, STR RO 481 || DINALVA SILVA DOS SANTOS - SITIO DOS ANJOS - BR 429, KM 1,5, LT 24, GB 11, STR BR 429 SENT/SERING || DINALVA SILVA DOS SANTOS - CHACARA BOA SORTE - LH 25 (MORTA), KM 6, LT 08, GB 5, STR RO 481 || DINALVA SILVA DOS SANTOS - SITIO DOS ANJOS - BR 429, KM 1,5, LT 24, GB 11, STR BR 429 SENT/SERING</t>
+          <t>JOILMA GLEICE SCHIAVI GOMES - FAZENDA PANTANEIRA - LH 22-C, KM 30, GB TERRA FIRME, STR MANOEL CORREIA</t>
         </is>
       </c>
     </row>
@@ -594,12 +594,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>+55 69 984521725</t>
+          <t>+55 69 984727071</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CAMILA CAROLINA FERREIRA CRUZ CHOQUE - RANCHO BRASIL - LH 82 NORTE, KM 1, LT 15E, GB 13, STR CHACAREIRO</t>
+          <t>JOILMA GLEICE SCHIAVI GOMES - FAZENDA PANTANEIRA - LH 22-C, KM 30, GB TERRA FIRME, STR MANOEL CORREIA</t>
         </is>
       </c>
     </row>
@@ -611,29 +611,29 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>+55 69 984528653</t>
+          <t>+55 69 984753371</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>VANDERLEI DE OLIVEIRA CORDEIRO - SITIO SOLO RICO - LH 86 SUL, KM 20, LT 01B, GB 01, STR RO 481</t>
+          <t>CACILDA RIBEIRO ALVES - SITIO ESTRELA DALVA - LH 90 SUL, KM 6, LT 47 -D, GB 03, STR RO 481, DESMEMBRADO</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Enviado</t>
+          <t>Número inválido</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>+55 69 984680406</t>
+          <t>+55 69 984761436</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>JOILMA GLEICE SCHIAVI GOMES - FAZENDA PANTANEIRA - LH 22-C, KM 30, GB TERRA FIRME, STR MANOEL CORREIA</t>
+          <t>DILSON DE MATTIA - nan - ROD. RO 481, KM 5, LT 09, GB 04, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -645,12 +645,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>+55 69 984727071</t>
+          <t>+55 69 984794012</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>JOILMA GLEICE SCHIAVI GOMES - FAZENDA PANTANEIRA - LH 22-C, KM 30, GB TERRA FIRME, STR MANOEL CORREIA</t>
+          <t>GILBERTO BARBOSA SILVA - CHACARA LAÇO FORTE III - LH 74 SUL, KM 1, LT 008, GB 007, STR BR 429 SENT/SERING, DESMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -662,12 +662,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>+55 69 984742472</t>
+          <t>+55 69 984890989</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>PLINIO FUNKLER - SITIO RECANTO ALEGRE - BR 429, KM 3,8, LT 13, 15 E 17, GB 14, STR BR 429 SENT/SERING, ROD BR 429 SENTIDO SERINGUEIRAS</t>
+          <t>GILMARA BORGES DA SILVA - CHACARA BORGES - LH 78 SUL, KM 1, LT 16, GB 5, STR BR 429 SENT/SERING, SUL</t>
         </is>
       </c>
     </row>
@@ -679,29 +679,29 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>+55 69 984753371</t>
+          <t>+55 69 984896588</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>CACILDA RIBEIRO ALVES - SITIO ESTRELA DALVA - LH 90 SUL, KM 6, LT 47 -D, GB 03, STR RO 481, DESMEMBRADO</t>
+          <t>VALDIVIO BONFIM DOS REIS - CH PEDACINHO DO CEU - BR 429, KM 1,5, LT 5B, GB 12, STR BR 429 SENT/ALV</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Número inválido</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>+55 69 984761436</t>
+          <t>+55 69 992015981</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>DILSON DE MATTIA - nan - ROD. RO 481, KM 5, LT 09, GB 04, STR RO 481</t>
+          <t>SANDRA ROMUALDA RAMOS - nan - LH 94 NORTE, KM 11, LT 78, GB 09, STR RO 481, DESMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -713,12 +713,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>+55 69 984786585</t>
+          <t>+55 69 992037445</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>JOSE PAULO DA SILVA - SITIO DOIS VIZINHOS - LH 90 SUL, KM 8, LT 66A, GB 02, STR RO 481</t>
+          <t>JOSE PEREIRA MADEIRA - SITIO BOM JESUS - ROD. RO 481, KM 9, LT 7, GB 10, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -730,12 +730,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>+55 69 984794012</t>
+          <t>+55 69 992191613</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>GILBERTO BARBOSA SILVA - CHACARA LAÇO FORTE III - LH 74 SUL, KM 1, LT 008, GB 007, STR BR 429 SENT/SERING, DESMEMBRADO</t>
+          <t>HEBERSON DA SILVA JULIO - SITIO DOIS IRMAO - LH 09 SUL, KM 8, LT 56, GB 01, STR BR 429 SENT/SERING</t>
         </is>
       </c>
     </row>
@@ -747,12 +747,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>+55 69 984794502</t>
+          <t>+55 69 992305466</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>JOAO BATISTA DE SOUZA - nan - BR 429, KM 1, LT 6, GB 12, STR BR 429 SENT/ALV, CHACAR FUNDIARIA</t>
+          <t>CAMILA CAROLINA FERREIRA CRUZ CHOQUE - RANCHO BRASIL - LH 82 NORTE, KM 1, LT 15E, GB 13, STR CHACAREIRO</t>
         </is>
       </c>
     </row>
@@ -764,12 +764,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>+55 69 984890989</t>
+          <t>+55 69 992310723</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>GILMARA BORGES DA SILVA - CHACARA BORGES - LH 78 SUL, KM 1, LT 16, GB 5, STR BR 429 SENT/SERING, SUL</t>
+          <t>VITOR MANOEL PRUDENCIO DA SILVA - ESTANCIA PRUDENCIO - BR 429, KM 5,5, LT 33, GB 10, STR BR 429 SENT/ALV</t>
         </is>
       </c>
     </row>
@@ -781,12 +781,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>+55 69 984896588</t>
+          <t>+55 69 992338411</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>VALDIVIO BONFIM DOS REIS - CH PEDACINHO DO CEU - BR 429, KM 1,5, LT 5B, GB 12, STR BR 429 SENT/ALV</t>
+          <t>ADAIR DE FREITAS - SITIO BOA ESPERANÇA - LH 25 (MORTA), KM 3, LT 13A, GB 05, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -798,97 +798,97 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>+55 69 992006355</t>
+          <t>+55 69 992376817</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>JOSE DIOGO OLIVEIRA DOS SANTOS - SITIO SAO JOSE - LH 86 SUL, KM 10, LT 82A REMANESCENTE, GB 3, STR RO 481</t>
+          <t>ELAINE RODRIGUES SAQUETTE - SITIO SANTA ROSA - LH 86 SUL, KM 10, LT 81, GB 04, STR RO 481, L.D</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Número inválido</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>+55 69 992015981</t>
+          <t>+55 69 992380140</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>SANDRA ROMUALDA RAMOS - nan - LH 94 NORTE, KM 11, LT 78, GB 09, STR RO 481, DESMEMBRADO</t>
+          <t>CICERA DA SILVA PEREIRA - SITIO JESUS MARIA - LH 86 SUL, KM 14, LT 110, GB 03, STR RO 481, L.E APOS TRAVESSAO</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Enviado</t>
+          <t>Número inválido</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>+55 69 992037445</t>
+          <t>+55 69 992390695</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>JOSE PEREIRA MADEIRA - SITIO BOM JESUS - ROD. RO 481, KM 9, LT 7, GB 10, STR RO 481</t>
+          <t>CACILDA RIBEIRO ALVES - SITIO ESTRELA DALVA - LH 90 SUL, KM 6, LT 47 -D, GB 03, STR RO 481, DESMEMBRADO</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Enviado</t>
+          <t>Número inválido</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>+55 69 992191613</t>
+          <t>+55 69 992480618</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>HEBERSON DA SILVA JULIO - SITIO DOIS IRMAO - LH 09 SUL, KM 8, LT 56, GB 01, STR BR 429 SENT/SERING</t>
+          <t>MARLI DOS SANTOS FERREIRA - nan - ROD. RO 481, KM 9, LT 09B, GB 10, STR RO 481, L.E</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Número inválido</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>+55 69 992263210</t>
+          <t>+55 69 992495947</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>PLINIO FUNKLER - SITIO RECANTO ALEGRE - BR 429, KM 3,8, LT 13, 15 E 17, GB 14, STR BR 429 SENT/SERING, ROD BR 429 SENTIDO SERINGUEIRAS</t>
+          <t>LUCIANO GOMES RIBEIRO - CHACARA L A - LH 25, KM 8, LT 44, GB 01, STR BR 429 SENT/SERING || LUCIANO GOMES RIBEIRO - CHACARA L A - LH 25, KM 8, LT 44, GB 01, STR BR 429 SENT/SERING || LUCIANO GOMES RIBEIRO - CHACARA L A - LH 25, KM 8, LT 44, GB 01, STR BR 429 SENT/SERING</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Número inválido</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>+55 69 992289248</t>
+          <t>+55 69 992504159</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>JOSE ANTONIO BARBOSA - SITIO BOM JESUS DA LAPA - LH 94 SUL, KM 7, LT 57 E 55, GB 02, STR RO 481, DESMEMBRADO</t>
+          <t>MANOEL JOSE DE LIMA - SITIO BOA FE - LH 98 SUL, KM 7,5, LT 46, GB 10, STR RO 481, DESMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -900,12 +900,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>+55 69 992305466</t>
+          <t>+55 69 992515775</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CAMILA CAROLINA FERREIRA CRUZ CHOQUE - RANCHO BRASIL - LH 82 NORTE, KM 1, LT 15E, GB 13, STR CHACAREIRO</t>
+          <t>CIRO CARDOSO CHICATTO - FAZENDA VITORIA - LH 50 SUL, KM 90, LT 1,2,3,4,5,7,9,11,13 E 15, GB 11, STR PRIMAVERA</t>
         </is>
       </c>
     </row>
@@ -917,12 +917,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>+55 69 992310723</t>
+          <t>+55 69 992571440</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>VITOR MANOEL PRUDENCIO DA SILVA - ESTANCIA PRUDENCIO - BR 429, KM 5,5, LT 33, GB 10, STR BR 429 SENT/ALV</t>
+          <t>JOSIAS BENTO DA SILVA - CH - ROD. RO 481, KM 15, LT 4, GB 8, STR RO 481 || JOSIAS BENTO DA SILVA - CH - ROD. RO 481, KM 15, LT 4, GB 8, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -934,12 +934,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>+55 69 992338411</t>
+          <t>+55 69 992581244</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ADAIR DE FREITAS - SITIO BOA ESPERANÇA - LH 25 (MORTA), KM 3, LT 13A, GB 05, STR RO 481</t>
+          <t>RONDRE PETERS DA SILVA DE JESUS - SITIO SAO FRANCISCO - LH 98 NORTE, KM 10, LT 50, GB 15, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -951,12 +951,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>+55 69 992376817</t>
+          <t>+55 69 992684151</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ELAINE RODRIGUES SAQUETTE - SITIO SANTA ROSA - LH 86 SUL, KM 10, LT 81, GB 04, STR RO 481, L.D</t>
+          <t>JUAN FELIPE TAVARES HENKERT - SITIO RECANTO - BR 429, KM 23, LT 144A, GB 01, STR BR 429 SENT/SERING</t>
         </is>
       </c>
     </row>
@@ -968,12 +968,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>+55 69 992380140</t>
+          <t>+55 69 992714223</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>CICERA DA SILVA PEREIRA - SITIO JESUS MARIA - LH 86 SUL, KM 14, LT 110, GB 03, STR RO 481, L.E APOS TRAVESSAO</t>
+          <t>EUGENIO SILVA DE ALMEIDA - SITIO 2 F - LH 74 SUL, KM 16, LT 138 A, GB 06, STR BR 429 SENT/SERING</t>
         </is>
       </c>
     </row>
@@ -985,29 +985,29 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>+55 69 992390695</t>
+          <t>+55 69 992721394</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>CACILDA RIBEIRO ALVES - SITIO ESTRELA DALVA - LH 90 SUL, KM 6, LT 47 -D, GB 03, STR RO 481, DESMEMBRADO</t>
+          <t>GRAZIELY FERNANDA AUGUSTA NOGUEIRA - SITIO UNIAO - LH 82 SUL, KM 17, LT 119 A, GB 05, STR RO 481</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Número inválido</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>+55 69 992480618</t>
+          <t>+55 69 992742030</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>MARLI DOS SANTOS FERREIRA - nan - ROD. RO 481, KM 9, LT 09B, GB 10, STR RO 481, L.E</t>
+          <t>EDILSON MIRANDA DA SILVA - SITIO BELA VISTA - LH 86 SUL, KM 9, LT 78, GB 03, STR RO 481, L E. FUNDO DA IGREJA ASSEMBLEIA APOS CAMPO.</t>
         </is>
       </c>
     </row>
@@ -1019,12 +1019,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>+55 69 992495947</t>
+          <t>+55 69 992839373</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>LUCIANO GOMES RIBEIRO - CHACARA L A - LH 25, KM 8, LT 44, GB 01, STR BR 429 SENT/SERING || LUCIANO GOMES RIBEIRO - CHACARA L A - LH 25, KM 8, LT 44, GB 01, STR BR 429 SENT/SERING || LUCIANO GOMES RIBEIRO - CHACARA L A - LH 25, KM 8, LT 44, GB 01, STR BR 429 SENT/SERING</t>
+          <t>CIRO CARDOSO CHICATTO - FAZENDA VITORIA - LH 50 SUL, KM 90, LT 1,2,3,4,5,7,9,11,13 E 15, GB 11, STR PRIMAVERA</t>
         </is>
       </c>
     </row>
@@ -1036,29 +1036,29 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>+55 69 992504159</t>
+          <t>+55 69 992869860</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>MANOEL JOSE DE LIMA - SITIO BOA FE - LH 98 SUL, KM 7,5, LT 46, GB 10, STR RO 481, DESMEMBRADO</t>
+          <t>EUGENIO SILVA DE ALMEIDA - SITIO 2 F - LH 74 SUL, KM 16, LT 138 A, GB 06, STR BR 429 SENT/SERING</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Enviado</t>
+          <t>Número inválido</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>+55 69 992515220</t>
+          <t>+55 69 992879674</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>GLEYSON CARDOSO FIDELIS RAMOS - SITIO DINIZ - BR 429, KM 0, LT 18 REM, GB 11, STR BR 429 SENT/SERING</t>
+          <t>JOAO MARIA RODRIGUES - SITIO SAO MARCOS - LH 74 SUL, KM 6,2, LT 22 E 23, GB 07, STR BR 429 SENT/SERING, APOS O BOTECO DO NENO</t>
         </is>
       </c>
     </row>
@@ -1070,12 +1070,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>+55 69 992515775</t>
+          <t>+55 69 992912652</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>CIRO CARDOSO CHICATTO - FAZENDA VITORIA - LH 50 SUL, KM 90, LT 1,2,3,4,5,7,9,11,13 E 15, GB 11, STR PRIMAVERA</t>
+          <t>DILSON DE MATTIA - nan - ROD. RO 481, KM 5, LT 09, GB 04, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -1087,12 +1087,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>+55 69 992528058</t>
+          <t>+55 69 992936682</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>CRISTIANE EISING DE ALMEIDA - CHACARA SAO JOSE - LH 94 SUL, KM 12, LT 47-A, GB 01, STR RO 481</t>
+          <t>CLEBERSON MACEDO BARROS - SITIO MACEDO - LH 90 SUL, KM 16, LT 128, GB 2, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -1104,12 +1104,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>+55 69 992571440</t>
+          <t>+55 69 992962784</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>JOSIAS BENTO DA SILVA - CH - ROD. RO 481, KM 15, LT 4, GB 8, STR RO 481 || JOSIAS BENTO DA SILVA - CH - ROD. RO 481, KM 15, LT 4, GB 8, STR RO 481</t>
+          <t>EUGENIO SILVA DE ALMEIDA - SITIO 2 F - LH 74 SUL, KM 16, LT 138 A, GB 06, STR BR 429 SENT/SERING</t>
         </is>
       </c>
     </row>
@@ -1121,12 +1121,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>+55 69 992581244</t>
+          <t>+55 69 993026972</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>RONDRE PETERS DA SILVA DE JESUS - SITIO SAO FRANCISCO - LH 98 NORTE, KM 10, LT 50, GB 15, STR RO 481</t>
+          <t>ROSINEIDE OLIVEIRA DA SILVA - SITIO SAO JOSE - LH 86 SUL, KM 10, LT 82A REMANESCENTE, GB 3, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -1138,12 +1138,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>+55 69 992684151</t>
+          <t>+55 69 993161087</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>JUAN FELIPE TAVARES HENKERT - SITIO RECANTO - BR 429, KM 23, LT 144A, GB 01, STR BR 429 SENT/SERING</t>
+          <t>HILTON DE JESUS SOUZA - CHACARA BOM JESUS - LH 78 SUL, KM 12, LT 69, GB 6, STR BR 429 SENT/SERING, DESMEMBRADA</t>
         </is>
       </c>
     </row>
@@ -1155,29 +1155,29 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>+55 69 992714223</t>
+          <t>+55 69 993185430</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>EUGENIO SILVA DE ALMEIDA - SITIO 2 F - LH 74 SUL, KM 16, LT 138 A, GB 06, STR BR 429 SENT/SERING</t>
+          <t>EILANE GONÇALVES DE ALMEIDA - CHACARA TRES IRMAS - LH 86 SUL, KM 10, LT 86, GB 3, STR RO 481</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Enviado</t>
+          <t>Número inválido</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>+55 69 992721394</t>
+          <t>+55 69 993449821</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>GRAZIELY FERNANDA AUGUSTA NOGUEIRA - SITIO UNIAO - LH 82 SUL, KM 17, LT 119 A, GB 05, STR RO 481</t>
+          <t>EILANE GONÇALVES DE ALMEIDA - CHACARA TRES IRMAS - LH 86 SUL, KM 10, LT 86, GB 3, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -1189,12 +1189,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>+55 69 992742030</t>
+          <t>+55 69 993624344</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>EDILSON MIRANDA DA SILVA - SITIO BELA VISTA - LH 86 SUL, KM 9, LT 78, GB 03, STR RO 481, L E. FUNDO DA IGREJA ASSEMBLEIA APOS CAMPO.</t>
+          <t>RONDRE PETERS DA SILVA DE JESUS - SITIO SAO FRANCISCO - LH 98 NORTE, KM 10, LT 50, GB 15, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -1206,12 +1206,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>+55 69 992855880</t>
+          <t>+55 69 993683661</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>ANA PAULA BRITO DE ALMEIDA - SITIO PRIMAVERA - LH 58 SUL, KM 7, LT 10,12,14 E 16, GB 9, STR PRIMAVERA, DESMEMBRADO</t>
+          <t>FERNANDO ANER DE OLIVEIRA - SITIO PAI E FILHO - LH 78 SUL, KM 9,5, LT 76 REM E 76-C, GB 05, STR BR 429 SENT/ALV</t>
         </is>
       </c>
     </row>
@@ -1223,29 +1223,29 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>+55 69 992869860</t>
+          <t>+55 69 993686605</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>EUGENIO SILVA DE ALMEIDA - SITIO 2 F - LH 74 SUL, KM 16, LT 138 A, GB 06, STR BR 429 SENT/SERING</t>
+          <t>MOACIR ROMUALDA RAMOS TUME - SITIO BOA ESPERANÇA - LH 94 NORTE, KM 11, LT 78, GB 09, STR RO 481, DESMEMBRADO</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Número inválido</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>+55 69 992879674</t>
+          <t>+55 69 993705091</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>JOAO MARIA RODRIGUES - SITIO SAO MARCOS - LH 74 SUL, KM 6,2, LT 22 E 23, GB 07, STR BR 429 SENT/SERING, APOS O BOTECO DO NENO</t>
+          <t>SILVANA APARECIDA CANHIN SILVA - CHACARA BOM FUTURO - BR 429, KM 2, LT 11-A2, GB 11, STR BR 429 SENT/ALV, L.D FUNDIARIA</t>
         </is>
       </c>
     </row>
@@ -1257,12 +1257,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>+55 69 992912652</t>
+          <t>+55 69 993805836</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>DILSON DE MATTIA - nan - ROD. RO 481, KM 5, LT 09, GB 04, STR RO 481</t>
+          <t>GRAZIELY FERNANDA AUGUSTA NOGUEIRA - SITIO UNIAO - LH 82 SUL, KM 17, LT 119 A, GB 05, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -1274,29 +1274,29 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>+55 69 992936682</t>
+          <t>+55 69 993897941</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>CLEBERSON MACEDO BARROS - SITIO MACEDO - LH 90 SUL, KM 16, LT 128, GB 2, STR RO 481</t>
+          <t>RUTIELE TAVARES HENKERT - SITIO DA FAMILIA SOARES - BR 429, KM 25, LT 143A, GB 1, STR BR 429 SENT/SERING</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Enviado</t>
+          <t>Número inválido</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>+55 69 992962784</t>
+          <t>+55 69 993904647</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>EUGENIO SILVA DE ALMEIDA - SITIO 2 F - LH 74 SUL, KM 16, LT 138 A, GB 06, STR BR 429 SENT/SERING</t>
+          <t>VALDIVIO BONFIM DOS REIS - CH PEDACINHO DO CEU - BR 429, KM 1,5, LT 5B, GB 12, STR BR 429 SENT/ALV</t>
         </is>
       </c>
     </row>
@@ -1308,12 +1308,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>+55 69 992962876</t>
+          <t>+55 69 993915285</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>WASHINGTON BRASSAROTO SANDOS - SITIO SANTA INES - ROD. RO 481, KM 3, LT 009, GB 04, STR RO 481, DESMEMBRADO</t>
+          <t>KARINA TYEMI CARVALHO - FAZENDA SETE PONTE - LH 22-C-SETE PONTES, KM 5, LT 33,36 E 39, GB TERRA FIRME, STR MANOEL CORREIA, BR 429 KM 155 || KARINA TYEMI CARVALHO - FAZENDA SETE PONTE - LH 22-C-SETE PONTES, KM 5, LT 33,36 E 39, GB TERRA FIRME, STR MANOEL CORREIA, BR 429 KM 155</t>
         </is>
       </c>
     </row>
@@ -1325,12 +1325,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>+55 69 993026972</t>
+          <t>+55 69 993949196</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>ROSINEIDE OLIVEIRA DA SILVA - SITIO SAO JOSE - LH 86 SUL, KM 10, LT 82A REMANESCENTE, GB 3, STR RO 481</t>
+          <t>JULIO GUSTAVO PEREIRA DE QUEIROZ - CHACARA BOA ESPERANÇA - ROD. RO 481, KM 2,5, LT 14, GB 4, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -1342,12 +1342,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>+55 69 993161087</t>
+          <t>+55 69 993966710</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>HILTON DE JESUS SOUZA - CHACARA BOM JESUS - LH 78 SUL, KM 12, LT 69, GB 6, STR BR 429 SENT/SERING, DESMEMBRADA</t>
+          <t>SIDNEY FERREIRA DE SOUZA - FAZENDA BOA ESPERANÇA - LH 74 SUL, KM 48, LT 21, GB RIO BRANCO, STR PRIMAVERA || SIDNEY FERREIRA DE SOUZA - SITIO DOIS IRMAOS - LH 78 SUL, KM 20, LT 146, GB 05, STR BR 429 SENT/SERING</t>
         </is>
       </c>
     </row>
@@ -1359,12 +1359,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>+55 69 993185430</t>
+          <t>+55 69 996058487</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>EILANE GONÇALVES DE ALMEIDA - CHACARA TRES IRMAS - LH 86 SUL, KM 10, LT 86, GB 3, STR RO 481</t>
+          <t>LUCAS DOMINGOS DIAS - CHACARA SILVA - LH 82 SUL, KM 5, LT 39 A, GB 5, STR RO 481, DESMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -1376,12 +1376,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>+55 69 993449821</t>
+          <t>+55 69 999098974</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>EILANE GONÇALVES DE ALMEIDA - CHACARA TRES IRMAS - LH 86 SUL, KM 10, LT 86, GB 3, STR RO 481</t>
+          <t>LEONIDAS RAMOS DE SOUZA FILHO - SITIO RIO GRANDE - LH 90 SUL, KM 15,5, LT 123, GB 03, STR RO 481, SUL || LEONIDAS RAMOS DE SOUZA FILHO - CH BOA ESPERAÇA - LH 94 SUL, KM 12, LT 51 B, GB 1, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -1393,29 +1393,29 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>+55 69 993624344</t>
+          <t>+55 69 999146496</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>RONDRE PETERS DA SILVA DE JESUS - SITIO SAO FRANCISCO - LH 98 NORTE, KM 10, LT 50, GB 15, STR RO 481</t>
+          <t>EDILSON CAVALCANTE PROCOPIO - CHACARA PROCOPIO - LH 94 NORTE, KM 6,5, LT 24 - B1, GB 8, STR RO 481 || EDILSON CAVALCANTE PROCOPIO - CHACARA PROCOPIO - LH 94 NORTE, KM 6,5, LT 24 - B1, GB 8, STR RO 481</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Número inválido</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>+55 69 993683661</t>
+          <t>+55 69 999191109</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>FERNANDO ANER DE OLIVEIRA - SITIO PAI E FILHO - LH 78 SUL, KM 9,5, LT 76 REM E 76-C, GB 05, STR BR 429 SENT/ALV</t>
+          <t>LUCAS DOMINGOS DIAS - CHACARA SILVA - LH 82 SUL, KM 5, LT 39 A, GB 5, STR RO 481, DESMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -1427,12 +1427,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>+55 69 993686605</t>
+          <t>+55 69 999205960</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>MOACIR ROMUALDA RAMOS TUME - SITIO BOA ESPERANÇA - LH 94 NORTE, KM 11, LT 78, GB 09, STR RO 481, DESMEMBRADO</t>
+          <t>JOSMARIO DINIZ DE MATOS - SITIO BELA VISTA - ROD. RO 481, KM 8, LT 01, GB 10, STR RO 481, DESMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -1444,12 +1444,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>+55 69 993705091</t>
+          <t>+55 69 999222396</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>SILVANA APARECIDA CANHIN SILVA - CHACARA BOM FUTURO - BR 429, KM 2, LT 11-A2, GB 11, STR BR 429 SENT/ALV, L.D FUNDIARIA</t>
+          <t>LUIZ FELIPE SILVA - SITIO NORTE SUL - LH 94 SUL, KM 3, LT 14 C, 14D E 14 REMANESCENTE, GB 1, STR RO 481, L.E APOS ASSOCIAÇAO - FUNDIARIA</t>
         </is>
       </c>
     </row>
@@ -1461,12 +1461,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>+55 69 993805836</t>
+          <t>+55 69 999400839</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>GRAZIELY FERNANDA AUGUSTA NOGUEIRA - SITIO UNIAO - LH 82 SUL, KM 17, LT 119 A, GB 05, STR RO 481</t>
+          <t>TCHARLLIS SOUZA BRANDT - SITIO PARAISO - LH 98 SUL, KM 4, LT 76A, GB 10, STR RO 481, DESMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -1478,46 +1478,46 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>+55 69 993824598</t>
+          <t>+55 69 999404334</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>JOSE PAULO DA SILVA - SITIO DOIS VIZINHOS - LH 90 SUL, KM 8, LT 66A, GB 02, STR RO 481</t>
+          <t>ALEIDA DE OLIVEIRA - nan - LH 94 SUL, KM 13, LT 55, GB 01, STR RO 481, DESMEMBRADA CONFORME ESDRITURA DE PARTILHA</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Enviado</t>
+          <t>Número inválido</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>+55 69 993897941</t>
+          <t>+55 69 999462417</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>RUTIELE TAVARES HENKERT - SITIO DA FAMILIA SOARES - BR 429, KM 25, LT 143A, GB 1, STR BR 429 SENT/SERING</t>
+          <t>VALDEMAR CLAUDINO DOS SANTOS - SITIO GOIAS - LH 98 NORTE, KM 5, LT 17, GB 16, STR RO 481</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Número inválido</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>+55 69 993904647</t>
+          <t>+55 69 999668080</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>VALDIVIO BONFIM DOS REIS - CH PEDACINHO DO CEU - BR 429, KM 1,5, LT 5B, GB 12, STR BR 429 SENT/ALV</t>
+          <t>ADRIELSON CAUTULINO DE SOUZA - SITIO SANTA IZABEL - LH 94 SUL, KM 2,5, LT 10, GB 01, STR RO 481, DESMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -1529,12 +1529,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>+55 69 993915285</t>
+          <t>+55 69 999845726</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>KARINA TYEMI CARVALHO - FAZENDA SETE PONTE - LH 22-C-SETE PONTES, KM 5, LT 33,36 E 39, GB TERRA FIRME, STR MANOEL CORREIA, BR 429 KM 155 || KARINA TYEMI CARVALHO - FAZENDA SETE PONTE - LH 22-C-SETE PONTES, KM 5, LT 33,36 E 39, GB TERRA FIRME, STR MANOEL CORREIA, BR 429 KM 155</t>
+          <t>VALDETE GONÇALVES - SITIO BOA SORTE - LH 94 NORTE, KM 3, LT 13, GB 08, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -1546,401 +1546,10 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>+55 69 993949196</t>
+          <t>+55 69 999962491</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
-        <is>
-          <t>JULIO GUSTAVO PEREIRA DE QUEIROZ - CHACARA BOA ESPERANÇA - ROD. RO 481, KM 2,5, LT 14, GB 4, STR RO 481</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>+55 69 993966710</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>SIDNEY FERREIRA DE SOUZA - SITIO DOIS IRMAOS - LH 78 SUL, KM 20, LT 146, GB 05, STR BR 429 SENT/SERING || SIDNEY FERREIRA DE SOUZA - FAZENDA BOA ESPERANÇA - LH 74 SUL, KM 48, LT 21, GB RIO BRANCO, STR PRIMAVERA</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>+55 69 996058487</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>LUCAS DOMINGOS DIAS - CHACARA SILVA - LH 82 SUL, KM 5, LT 39 A, GB 5, STR RO 481, DESMEMBRADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>Número inválido</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>+55 69 999098974</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>LEONIDAS RAMOS DE SOUZA FILHO - SITIO RIO GRANDE - LH 90 SUL, KM 15,5, LT 123, GB 03, STR RO 481, SUL || LEONIDAS RAMOS DE SOUZA FILHO - CH BOA ESPERAÇA - LH 94 SUL, KM 12, LT 51 B, GB 1, STR RO 481</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>+55 69 999146496</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>EDILSON CAVALCANTE PROCOPIO - CHACARA PROCOPIO - LH 94 NORTE, KM 6,5, LT 24 - B1, GB 8, STR RO 481 || EDILSON CAVALCANTE PROCOPIO - CHACARA PROCOPIO - LH 94 NORTE, KM 6,5, LT 24 - B1, GB 8, STR RO 481</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>Número inválido</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>+55 69 999172504</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>EDICARLOS MASCARENHAS DE MORAIS - SITIO BOA VISTA - LH 78 SUL, KM 16, LT 120, GB 05, STR BR 429 SENT/SERING</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>+55 69 999191109</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>LUCAS DOMINGOS DIAS - CHACARA SILVA - LH 82 SUL, KM 5, LT 39 A, GB 5, STR RO 481, DESMEMBRADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>+55 69 999205960</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>JOSMARIO DINIZ DE MATOS - SITIO BELA VISTA - ROD. RO 481, KM 8, LT 01, GB 10, STR RO 481, DESMEMBRADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>+55 69 999214106</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>FABIANO ESTEVES DE ALMEIDA - SITIO DOIS IRMAOS - LH 86 SUL, KM 7, LT 61A, GB 4, STR RO 481, DESMENBRADO || FABIANO ESTEVES DE ALMEIDA - SITIO DOIS IRMAOS - LH 86 SUL, KM 7, LT 61A, GB 4, STR RO 481, DESMENBRADO || FABIANO ESTEVES DE ALMEIDA - SITIO DOIS IRMAOS - LH 86 SUL, KM 7, LT 61A, GB 4, STR RO 481, DESMENBRADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>+55 69 999222396</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>LUIZ FELIPE SILVA - SITIO NORTE SUL - LH 94 SUL, KM 3, LT 14 C, 14D E 14 REMANESCENTE, GB 1, STR RO 481, L.E APOS ASSOCIAÇAO - FUNDIARIA</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>+55 69 999265811</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>THIAGO WESTFAL STRELOW - FAZENDA MINEIRA - LH 70 SUL, KM 45, LT 13,14,15 E12, GB RIO BRANCO, STR PRIMAVERA || THIAGO WESTFAL STRELOW - FAZENDA MINEIRA - LH 70 SUL, KM 45, LT 13,14,15 E12, GB RIO BRANCO, STR PRIMAVERA</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>+55 69 999267106</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>MAURO PINHEIRO TORRES - CH PARAISO - BR 429, KM 3,5, LT PARTE DO 11 E 13, GB 012, STR BR 429 SENT/ALV</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>+55 69 999323391</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>DELINA VIANA PERES - SITIO VISTA ALEGRE - LH 94 SUL, KM 4,75, LT 19, GB 01, STR RO 481, DESMEMBRADO || DELINA VIANA PERES - SITIO VISTA ALEGRE - LH 94 SUL, KM 4,75, LT 19, GB 01, STR RO 481, DESMEMBRADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>+55 69 999400839</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>TCHARLLIS SOUZA BRANDT - SITIO PARAISO - LH 98 SUL, KM 4, LT 76A, GB 10, STR RO 481, DESMEMBRADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>+55 69 999404334</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>ALEIDA DE OLIVEIRA - nan - LH 94 SUL, KM 13, LT 55, GB 01, STR RO 481, DESMEMBRADA CONFORME ESDRITURA DE PARTILHA</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>Número inválido</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>+55 69 999462417</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>VALDEMAR CLAUDINO DOS SANTOS - SITIO GOIAS - LH 98 NORTE, KM 5, LT 17, GB 16, STR RO 481</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>+55 69 999544601</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>DIEGO SANTANA DA CRUZ - SITIO TRES IRMAOS - LH 82 NORTE, KM 2,5, LT 24, GB 12, STR CHACAREIRO || DIEGO SANTANA DA CRUZ - CHACARA CUIABANA - LH 78 SUL, KM 20, LT 148A, GB 05, STR PRIMAVERA</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>+55 69 999612515</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>WASHINGTON BRASSAROTO SANDOS - SITIO SANTA INES - ROD. RO 481, KM 3, LT 009, GB 04, STR RO 481, DESMEMBRADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>+55 69 999623379</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>WASHINGTON BRASSAROTO SANDOS - SITIO SANTA INES - ROD. RO 481, KM 3, LT 009, GB 04, STR RO 481, DESMEMBRADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>+55 69 999668080</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>ADRIELSON CAUTULINO DE SOUZA - SITIO SANTA IZABEL - LH 94 SUL, KM 2,5, LT 10, GB 01, STR RO 481, DESMEMBRADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>+55 69 999790896</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>MAURO PINHEIRO TORRES - CH PARAISO - BR 429, KM 3,5, LT PARTE DO 11 E 13, GB 012, STR BR 429 SENT/ALV</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>+55 69 999845726</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>VALDETE GONÇALVES - SITIO BOA SORTE - LH 94 NORTE, KM 3, LT 13, GB 08, STR RO 481</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>+55 69 999960352</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>JOSE ANTONIO BARBOSA - SITIO BOM JESUS DA LAPA - LH 94 SUL, KM 7, LT 57 E 55, GB 02, STR RO 481, DESMEMBRADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>+55 69 999962491</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
         <is>
           <t>ALEX JACINTO DE SOUZA - CHACARA D.E.B - ROD. RO 481, KM 10, LT 16-B-1 E 14 REMANECENTE, GB 02, STR RO 481, FUNDIARIA, ACESSO LH 90 APOS PONTE</t>
         </is>

</xml_diff>

<commit_message>
Adiconado outros animais inadimplentes
</commit_message>
<xml_diff>
--- a/BancoProd.xlsx
+++ b/BancoProd.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,17 +453,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Enviado</t>
+          <t>Número inválido</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>+55 69 36421238</t>
+          <t>+55 00 000000000</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CLAUDIO DA SILVA - SITIO DUAS IRMAS - LH 78 SUL, KM 18, LT 130-A, GB 05, STR BR 429 SENT/SERING || EDIVALDO CARLOS DE OLIVEIRA - ST. FLOR DA MATA - LH 78 SUL, KM 20, LT 144, GB 05, STR BR 429 SENT/SERING || CLAUDIO DA SILVA - SITIO DUAS IRMAS - LH 78 SUL, KM 18, LT 130-A, GB 05, STR BR 429 SENT/SERING || CLAUDIO DA SILVA - SITIO DUAS IRMAS - LH 78 SUL, KM 18, LT 130-A, GB 05, STR BR 429 SENT/SERING</t>
+          <t>ATAIDE PEREIRA DE SOUZA - 110032005214 - LH 82 SUL, KM 6, LT 33, GB 5, STR RO 481, ENFRENTE O TANQUE DE LEITE</t>
         </is>
       </c>
     </row>
@@ -475,12 +475,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>+55 69 984266737</t>
+          <t>+55 45 998529397</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>JORGE ALVES RODRIGUES - CHACARA BANDEIRA BRANCA - LH 82 SUL, KM 8, LT 56, GB 4, STR RO 481, DEMEMBRADO</t>
+          <t>VALDECIR BORBA - 1100320054746 - LH 82 SUL, KM 7, LT 37B 35A1, GB 05, STR RO 481, L.D FUNDIARIA || VALDECIR BORBA - 1100320055366 - LH 25 (MORTA), KM 2, LT 01 A, GB 05, STR RO 481 || VALDECIR BORBA - 1100320052950 - LH 82 SUL, KM 6,5, LT 39, GB 05, STR RO 481 || VALDECIR BORBA - 1100320053037 - LH 25 (MORTA), KM 1, LT 42-C, GB 11, STR RO 481, L.D</t>
         </is>
       </c>
     </row>
@@ -492,12 +492,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>+55 69 984313304</t>
+          <t>+55 69 981149241</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ROSA GRAZIELE OLIVEIRA SOUZA CRAUSE - SITIO CATARINA - LH 98 NORTE, KM 11,5, LT 38-B1, GB 16, STR RO 481, TRAVESSAO DA 94 PARA 98 || ROSA GRAZIELE OLIVEIRA SOUZA CRAUSE - SITIO BOM SUCESSO - LH 94 NORTE, KM 4, LT 15, GB 08, STR RO 481, L.E</t>
+          <t>LUIS REGAÇONE - 1100320051247 - LH 86 SUL, KM 12, LT 100, GB 03, STR RO 481, DESMENBRAMDO</t>
         </is>
       </c>
     </row>
@@ -509,12 +509,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>+55 69 984397155</t>
+          <t>+55 69 981207921</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>LUCIA PEREIRA DOS SANTOS - SITIO TERRA ROXA - ROD. RO 481, KM 17, LT 3, GB RIO BRANCO, STR RO 481, DESMEMBRADO</t>
+          <t>LUIS REGAÇONE - 1100320051247 - LH 86 SUL, KM 12, LT 100, GB 03, STR RO 481, DESMENBRAMDO</t>
         </is>
       </c>
     </row>
@@ -526,12 +526,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>+55 69 984449468</t>
+          <t>+55 69 984096742</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>DINALVA SILVA DOS SANTOS - SITIO DOS ANJOS - BR 429, KM 1,5, LT 24, GB 11, STR BR 429 SENT/SERING || DINALVA SILVA DOS SANTOS - CHACARA BOA SORTE - LH 25 (MORTA), KM 6, LT 08, GB 5, STR RO 481 || JAIR SILVA GOMES - CHACARA BOA SORTE - LH 25 (MORTA), KM 6, LT 08, GB 5, STR RO 481 || DINALVA SILVA DOS SANTOS - SITIO DOS ANJOS - BR 429, KM 1,5, LT 24, GB 11, STR BR 429 SENT/SERING || DINALVA SILVA DOS SANTOS - CHACARA BOA SORTE - LH 25 (MORTA), KM 6, LT 08, GB 5, STR RO 481 || DINALVA SILVA DOS SANTOS - SITIO DOS ANJOS - BR 429, KM 1,5, LT 24, GB 11, STR BR 429 SENT/SERING || DINALVA SILVA DOS SANTOS - CHACARA BOA SORTE - LH 25 (MORTA), KM 6, LT 08, GB 5, STR RO 481</t>
+          <t>LUCIANO KOVALCHUK - 1100320054840 - LH 78 SUL, KM 1, LT 29C , GB 11, STR BR 429 SENT/SERING || LUCIANO KOVALCHUK - 1100320054840 - LH 78 SUL, KM 1, LT 29C , GB 11, STR BR 429 SENT/SERING</t>
         </is>
       </c>
     </row>
@@ -543,12 +543,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>+55 69 984521725</t>
+          <t>+55 69 984101481</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CAMILA CAROLINA FERREIRA CRUZ CHOQUE - RANCHO BRASIL - LH 82 NORTE, KM 1, LT 15E, GB 13, STR CHACAREIRO</t>
+          <t>NIRALVA DE OLIVEIRA SILVA - 1100320054474 - LH 74 SUL, KM 8,5, LT 90, GB 9, STR BR 429 SENT/SERING, DESMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -560,12 +560,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>+55 69 984528653</t>
+          <t>+55 69 984230843</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>VANDERLEI DE OLIVEIRA CORDEIRO - SITIO SOLO RICO - LH 86 SUL, KM 20, LT 01B, GB 01, STR RO 481</t>
+          <t>ONEIDA DE LIMA QUEIROZ - 1100320054423 - BR 429, KM 9, LT 20-A, GB 14, STR BR 429 SENT/SERING, L.D APOS IG.ASSEMBLEIA</t>
         </is>
       </c>
     </row>
@@ -577,12 +577,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>+55 69 984680406</t>
+          <t>+55 69 984396694</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>JOILMA GLEICE SCHIAVI GOMES - FAZENDA PANTANEIRA - LH 22-C, KM 30, GB TERRA FIRME, STR MANOEL CORREIA</t>
+          <t>JESSICA VENANCIO DA SILVA - 1100320053723 - LH 98 NORTE, KM 5,5, LT 19, GB 16, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -594,12 +594,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>+55 69 984727071</t>
+          <t>+55 69 984421186</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>JOILMA GLEICE SCHIAVI GOMES - FAZENDA PANTANEIRA - LH 22-C, KM 30, GB TERRA FIRME, STR MANOEL CORREIA</t>
+          <t>CLARICE DE FATIMA SOARES NUNES - 110032005348 - BR 429, KM 5, LT 33, GB 11, STR BR 429 SENT/SERING</t>
         </is>
       </c>
     </row>
@@ -611,29 +611,29 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>+55 69 984753371</t>
+          <t>+55 69 984432856</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CACILDA RIBEIRO ALVES - SITIO ESTRELA DALVA - LH 90 SUL, KM 6, LT 47 -D, GB 03, STR RO 481, DESMEMBRADO</t>
+          <t>MANNEZA JORDANIA BERNARDES DE OLIVIERA - 1100320054862 - LH 82 SUL, KM 6, LT 33, GB 5, STR RO 481, DESMEMBRADO || MANNEZA JORDANIA BERNARDES DE OLIVIERA - 1100320054862 - LH 82 SUL, KM 6, LT 33, GB 5, STR RO 481, DESMEMBRADO</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Número inválido</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>+55 69 984761436</t>
+          <t>+55 69 984577024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>DILSON DE MATTIA - nan - ROD. RO 481, KM 5, LT 09, GB 04, STR RO 481</t>
+          <t>ONEIDA DE LIMA QUEIROZ - 1100320054423 - BR 429, KM 9, LT 20-A, GB 14, STR BR 429 SENT/SERING, L.D APOS IG.ASSEMBLEIA</t>
         </is>
       </c>
     </row>
@@ -645,12 +645,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>+55 69 984794012</t>
+          <t>+55 69 984591377</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>GILBERTO BARBOSA SILVA - CHACARA LAÇO FORTE III - LH 74 SUL, KM 1, LT 008, GB 007, STR BR 429 SENT/SERING, DESMEMBRADO</t>
+          <t>FLORIZA ALVES DE OLIVEIRA - 1100320054275 - LH 94 SUL, KM 9, LT 37, GB 1, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -662,12 +662,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>+55 69 984890989</t>
+          <t>+55 69 984735692</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>GILMARA BORGES DA SILVA - CHACARA BORGES - LH 78 SUL, KM 1, LT 16, GB 5, STR BR 429 SENT/SERING, SUL</t>
+          <t>LUIS DEOTI - 1100320053322 - BR 429, KM 2, LT 06, GB 11, STR BR 429 SENT/ALV || LUIS DEOTI - 1100320053322 - BR 429, KM 2, LT 06, GB 11, STR BR 429 SENT/ALV || LUIS DEOTI - 1100320053322 - BR 429, KM 2, LT 06, GB 11, STR BR 429 SENT/ALV</t>
         </is>
       </c>
     </row>
@@ -679,12 +679,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>+55 69 984896588</t>
+          <t>+55 69 984835481</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>VALDIVIO BONFIM DOS REIS - CH PEDACINHO DO CEU - BR 429, KM 1,5, LT 5B, GB 12, STR BR 429 SENT/ALV</t>
+          <t>SIDNEI BARBOSA SIMAS - 1100320054710 - LH 25 (MORTA), KM 1,5, LT 05, GB 05, STR BR 429 SENT/SERING</t>
         </is>
       </c>
     </row>
@@ -696,12 +696,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>+55 69 992015981</t>
+          <t>+55 69 984956474</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>SANDRA ROMUALDA RAMOS - nan - LH 94 NORTE, KM 11, LT 78, GB 09, STR RO 481, DESMEMBRADO</t>
+          <t>REMY CARDOSO XAVIER - 1100320054292 - LH 94 NORTE, KM 3,5, LT 25A, GB 9, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -713,12 +713,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>+55 69 992037445</t>
+          <t>+55 69 992035882</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>JOSE PEREIRA MADEIRA - SITIO BOM JESUS - ROD. RO 481, KM 9, LT 7, GB 10, STR RO 481</t>
+          <t>JUCELIO DA SILVA PLASTER - 1100320055033 - LH 90 SUL, KM 5, LT 39, GB 3, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -730,12 +730,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>+55 69 992191613</t>
+          <t>+55 69 992207327</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>HEBERSON DA SILVA JULIO - SITIO DOIS IRMAO - LH 09 SUL, KM 8, LT 56, GB 01, STR BR 429 SENT/SERING</t>
+          <t>FLORIZA ALVES DE OLIVEIRA - 1100320054275 - LH 94 SUL, KM 9, LT 37, GB 1, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -747,12 +747,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>+55 69 992305466</t>
+          <t>+55 69 992240030</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>CAMILA CAROLINA FERREIRA CRUZ CHOQUE - RANCHO BRASIL - LH 82 NORTE, KM 1, LT 15E, GB 13, STR CHACAREIRO</t>
+          <t>MILTON ROSA DE ALMEIDA - 1100320051189 - BR 429, KM 25, LT 22, STR BR 429 SENT/ALV, DESMENBRADO</t>
         </is>
       </c>
     </row>
@@ -764,12 +764,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>+55 69 992310723</t>
+          <t>+55 69 992247521</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>VITOR MANOEL PRUDENCIO DA SILVA - ESTANCIA PRUDENCIO - BR 429, KM 5,5, LT 33, GB 10, STR BR 429 SENT/ALV</t>
+          <t>ROSENILDO SANT'ANA NIENCK - 1100320053908 - LH 82 SUL, KM 22, LT 03, GB 02, STR BR 429 SENT/SERING</t>
         </is>
       </c>
     </row>
@@ -781,12 +781,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>+55 69 992338411</t>
+          <t>+55 69 992362662</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ADAIR DE FREITAS - SITIO BOA ESPERANÇA - LH 25 (MORTA), KM 3, LT 13A, GB 05, STR RO 481</t>
+          <t>VALDOIR LENZ PEREIRA - 1100320054850 - BR 429, KM 22, LT 99, GB 01, STR BR 429 SENT/SERING || VALDOIR LENZ PEREIRA - 1100320054850 - BR 429, KM 22, LT 99, GB 01, STR BR 429 SENT/SERING</t>
         </is>
       </c>
     </row>
@@ -798,12 +798,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>+55 69 992376817</t>
+          <t>+55 69 992393252</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ELAINE RODRIGUES SAQUETTE - SITIO SANTA ROSA - LH 86 SUL, KM 10, LT 81, GB 04, STR RO 481, L.D</t>
+          <t>MARIQUINHA PRICILIUS - 1100320054651 - LH 82 SUL, KM 7, LT 37, GB 5, STR RO 481, DESMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -815,12 +815,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>+55 69 992380140</t>
+          <t>+55 69 992393453</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>CICERA DA SILVA PEREIRA - SITIO JESUS MARIA - LH 86 SUL, KM 14, LT 110, GB 03, STR RO 481, L.E APOS TRAVESSAO</t>
+          <t>VALDIR RODRIGUES DA SILVA - 1100320051603 - BR 429, KM 10, LT 22, GB 06, STR BR 429 SENT/SERING, DESMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -832,29 +832,29 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>+55 69 992390695</t>
+          <t>+55 69 992480618</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>CACILDA RIBEIRO ALVES - SITIO ESTRELA DALVA - LH 90 SUL, KM 6, LT 47 -D, GB 03, STR RO 481, DESMEMBRADO</t>
+          <t>MARLI DOS SANTOS FERREIRA - 1100320054724 - ROD. RO 481, KM 9, LT 09B, GB 10, STR RO 481, L.E</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Número inválido</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>+55 69 992480618</t>
+          <t>+55 69 992519218</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>MARLI DOS SANTOS FERREIRA - nan - ROD. RO 481, KM 9, LT 09B, GB 10, STR RO 481, L.E</t>
+          <t>ONEIDA DE LIMA QUEIROZ - 1100320054423 - BR 429, KM 9, LT 20-A, GB 14, STR BR 429 SENT/SERING, L.D APOS IG.ASSEMBLEIA</t>
         </is>
       </c>
     </row>
@@ -866,12 +866,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>+55 69 992495947</t>
+          <t>+55 69 992526904</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>LUCIANO GOMES RIBEIRO - CHACARA L A - LH 25, KM 8, LT 44, GB 01, STR BR 429 SENT/SERING || LUCIANO GOMES RIBEIRO - CHACARA L A - LH 25, KM 8, LT 44, GB 01, STR BR 429 SENT/SERING || LUCIANO GOMES RIBEIRO - CHACARA L A - LH 25, KM 8, LT 44, GB 01, STR BR 429 SENT/SERING</t>
+          <t>CLERIO MATOS DE ASSIS - 1100320055346 - LH 78 SUL, KM 3,5, LT 38, GB 11, STR BR 429 SENT/SERING</t>
         </is>
       </c>
     </row>
@@ -883,12 +883,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>+55 69 992504159</t>
+          <t>+55 69 992682247</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>MANOEL JOSE DE LIMA - SITIO BOA FE - LH 98 SUL, KM 7,5, LT 46, GB 10, STR RO 481, DESMEMBRADO</t>
+          <t>JORGE PEREIRA DOS SANTOS - 110032005704 - ROD. RO 481, KM 14, LT 01, GB 01, STR RO 481, ACESSO PELA LH 94 SUL KM 01</t>
         </is>
       </c>
     </row>
@@ -900,12 +900,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>+55 69 992515775</t>
+          <t>+55 69 992739233</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CIRO CARDOSO CHICATTO - FAZENDA VITORIA - LH 50 SUL, KM 90, LT 1,2,3,4,5,7,9,11,13 E 15, GB 11, STR PRIMAVERA</t>
+          <t>DANDARA HORANA DE OLIVEIRA GORZA - 110032005118 - LH 86 SUL, KM 11, LT 85, GB 04, STR RO 481, L.D</t>
         </is>
       </c>
     </row>
@@ -917,12 +917,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>+55 69 992571440</t>
+          <t>+55 69 992759904</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>JOSIAS BENTO DA SILVA - CH - ROD. RO 481, KM 15, LT 4, GB 8, STR RO 481 || JOSIAS BENTO DA SILVA - CH - ROD. RO 481, KM 15, LT 4, GB 8, STR RO 481</t>
+          <t>ANTONIO MARCOS GOMES - 1100320054742 - BR 429, KM 9,5, LT 22, GB 10, STR BR 429 SENT/SERING, L.D ACESSO IGREJA CRISTA</t>
         </is>
       </c>
     </row>
@@ -934,12 +934,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>+55 69 992581244</t>
+          <t>+55 69 992817550</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>RONDRE PETERS DA SILVA DE JESUS - SITIO SAO FRANCISCO - LH 98 NORTE, KM 10, LT 50, GB 15, STR RO 481</t>
+          <t>DAVI FIGUEIRA DOS SANTOS - 1100320053116 - LH 86 SUL, KM 12, LT 98-A, GB 03, STR RO 481, L E || DAVI FIGUEIRA DOS SANTOS - 1100320053116 - LH 86 SUL, KM 12, LT 98-A, GB 03, STR RO 481, L E || DAVI FIGUEIRA DOS SANTOS - 1100320053116 - LH 86 SUL, KM 12, LT 98-A, GB 03, STR RO 481, L E</t>
         </is>
       </c>
     </row>
@@ -951,12 +951,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>+55 69 992684151</t>
+          <t>+55 69 992832220</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>JUAN FELIPE TAVARES HENKERT - SITIO RECANTO - BR 429, KM 23, LT 144A, GB 01, STR BR 429 SENT/SERING</t>
+          <t>GERALDO GONÇALVES BRANDAO - 1100320053570 - LH 74 NORTE, KM 4,5, LT 36, GB 14, STR BR 429 SENT/SERING, 2 TRAVESSAO</t>
         </is>
       </c>
     </row>
@@ -968,29 +968,29 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>+55 69 992714223</t>
+          <t>+55 69 992836615</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>EUGENIO SILVA DE ALMEIDA - SITIO 2 F - LH 74 SUL, KM 16, LT 138 A, GB 06, STR BR 429 SENT/SERING</t>
+          <t>OSMAR FERNANDO BORGES - 1100320054105 - BR 429, KM 23, LT 263, GB 01, STR BR 429 SENT/SERING</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Número inválido</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>+55 69 992721394</t>
+          <t>+55 69 992946955</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>GRAZIELY FERNANDA AUGUSTA NOGUEIRA - SITIO UNIAO - LH 82 SUL, KM 17, LT 119 A, GB 05, STR RO 481</t>
+          <t>PEDRO PAULO BOA MORTE VAZ - 1100320051525 - LH 09 SUL, KM 8, LT 51, GB 001, STR BR 429 SENT/SERING</t>
         </is>
       </c>
     </row>
@@ -1002,12 +1002,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>+55 69 992742030</t>
+          <t>+55 69 992972422</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>EDILSON MIRANDA DA SILVA - SITIO BELA VISTA - LH 86 SUL, KM 9, LT 78, GB 03, STR RO 481, L E. FUNDO DA IGREJA ASSEMBLEIA APOS CAMPO.</t>
+          <t>DALVACY DA PENHA - 1100320055056 - BR 429, KM 8, LT 46, GB 11, STR BR 429 SENT/SERING</t>
         </is>
       </c>
     </row>
@@ -1019,12 +1019,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>+55 69 992839373</t>
+          <t>+55 69 993026718</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>CIRO CARDOSO CHICATTO - FAZENDA VITORIA - LH 50 SUL, KM 90, LT 1,2,3,4,5,7,9,11,13 E 15, GB 11, STR PRIMAVERA</t>
+          <t>VALDIR RODRIGUES DA SILVA - 1100320051603 - BR 429, KM 10, LT 22, GB 06, STR BR 429 SENT/SERING, DESMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -1036,29 +1036,29 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>+55 69 992869860</t>
+          <t>+55 69 993039887</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>EUGENIO SILVA DE ALMEIDA - SITIO 2 F - LH 74 SUL, KM 16, LT 138 A, GB 06, STR BR 429 SENT/SERING</t>
+          <t>GILMAR ANDERSON DA SILVA - 1100320051755 - LH 98 SUL, KM 12, LT 12, GB 10, STR RO 481, ROD RO 481</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Número inválido</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>+55 69 992879674</t>
+          <t>+55 69 993139237</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>JOAO MARIA RODRIGUES - SITIO SAO MARCOS - LH 74 SUL, KM 6,2, LT 22 E 23, GB 07, STR BR 429 SENT/SERING, APOS O BOTECO DO NENO</t>
+          <t>ATAIDE PEREIRA DE SOUZA - 110032005214 - LH 82 SUL, KM 6, LT 33, GB 5, STR RO 481, ENFRENTE O TANQUE DE LEITE</t>
         </is>
       </c>
     </row>
@@ -1070,12 +1070,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>+55 69 992912652</t>
+          <t>+55 69 993185430</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>DILSON DE MATTIA - nan - ROD. RO 481, KM 5, LT 09, GB 04, STR RO 481</t>
+          <t>EILANE GONÇALVES DE ALMEIDA - 1100320054696 - LH 86 SUL, KM 10, LT 86, GB 3, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -1087,12 +1087,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>+55 69 992936682</t>
+          <t>+55 69 993207066</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>CLEBERSON MACEDO BARROS - SITIO MACEDO - LH 90 SUL, KM 16, LT 128, GB 2, STR RO 481</t>
+          <t>VALDECI TIMOTEO - 1100320204476 - LH 90 SUL, KM 7, LT 60-A3, GB 2, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -1104,12 +1104,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>+55 69 992962784</t>
+          <t>+55 69 993266509</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>EUGENIO SILVA DE ALMEIDA - SITIO 2 F - LH 74 SUL, KM 16, LT 138 A, GB 06, STR BR 429 SENT/SERING</t>
+          <t>ORLANDINO ALVES DE OLIVEIRA - 1100320054275 - LH 94 SUL, KM 9, LT 37, GB 1, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -1121,29 +1121,29 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>+55 69 993026972</t>
+          <t>+55 69 993277937</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>ROSINEIDE OLIVEIRA DA SILVA - SITIO SAO JOSE - LH 86 SUL, KM 10, LT 82A REMANESCENTE, GB 3, STR RO 481</t>
+          <t>DANDARA HORANA DE OLIVEIRA GORZA - 110032005118 - LH 86 SUL, KM 11, LT 85, GB 04, STR RO 481, L.D</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Enviado</t>
+          <t>Número inválido</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>+55 69 993161087</t>
+          <t>+55 69 993317270</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>HILTON DE JESUS SOUZA - CHACARA BOM JESUS - LH 78 SUL, KM 12, LT 69, GB 6, STR BR 429 SENT/SERING, DESMEMBRADA</t>
+          <t>SIRLENE LIZZI CAVALCANTE - 110032005135 - LH 86 SUL, KM 19, LT 149, 149-A, GB 004, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -1155,12 +1155,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>+55 69 993185430</t>
+          <t>+55 69 99340680</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>EILANE GONÇALVES DE ALMEIDA - CHACARA TRES IRMAS - LH 86 SUL, KM 10, LT 86, GB 3, STR RO 481</t>
+          <t>GUMERCINO MARTINS GUIMARAES - 1100320053577 - LH 90 NORTE- NOVENTINHA, KM 2, LT 20, GB 09, STR RO 481, DESMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>EILANE GONÇALVES DE ALMEIDA - CHACARA TRES IRMAS - LH 86 SUL, KM 10, LT 86, GB 3, STR RO 481</t>
+          <t>EILANE GONÇALVES DE ALMEIDA - 1100320054696 - LH 86 SUL, KM 10, LT 86, GB 3, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -1189,12 +1189,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>+55 69 993624344</t>
+          <t>+55 69 993617963</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>RONDRE PETERS DA SILVA DE JESUS - SITIO SAO FRANCISCO - LH 98 NORTE, KM 10, LT 50, GB 15, STR RO 481</t>
+          <t>ISAIAS STRELOW - 1100320051135 - LH 98 NORTE, KM 10, LT 34-A, GB 16, STR RO 481, DESMENBRADO</t>
         </is>
       </c>
     </row>
@@ -1206,12 +1206,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>+55 69 993683661</t>
+          <t>+55 69 993645351</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>FERNANDO ANER DE OLIVEIRA - SITIO PAI E FILHO - LH 78 SUL, KM 9,5, LT 76 REM E 76-C, GB 05, STR BR 429 SENT/ALV</t>
+          <t>MANOEL DE MATOS PEREIRA - 1100320055279 - ROD. RO 481, KM 15, LT 04, GB 08, STR RO 481, NO TRAVESSAO</t>
         </is>
       </c>
     </row>
@@ -1223,12 +1223,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>+55 69 993686605</t>
+          <t>+55 69 993780921</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>MOACIR ROMUALDA RAMOS TUME - SITIO BOA ESPERANÇA - LH 94 NORTE, KM 11, LT 78, GB 09, STR RO 481, DESMEMBRADO</t>
+          <t>JUCELIO DA SILVA PLASTER - 1100320055033 - LH 90 SUL, KM 5, LT 39, GB 3, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -1240,12 +1240,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>+55 69 993705091</t>
+          <t>+55 69 993851802</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>SILVANA APARECIDA CANHIN SILVA - CHACARA BOM FUTURO - BR 429, KM 2, LT 11-A2, GB 11, STR BR 429 SENT/ALV, L.D FUNDIARIA</t>
+          <t>MANOEL DE MATOS PEREIRA - 1100320055279 - ROD. RO 481, KM 15, LT 04, GB 08, STR RO 481, NO TRAVESSAO</t>
         </is>
       </c>
     </row>
@@ -1257,12 +1257,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>+55 69 993805836</t>
+          <t>+55 69 993860390</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>GRAZIELY FERNANDA AUGUSTA NOGUEIRA - SITIO UNIAO - LH 82 SUL, KM 17, LT 119 A, GB 05, STR RO 481</t>
+          <t>RAIMUNDO DA CONCEIÇAO SA - 1100320054133 - BR 429, KM 7,5, LT 20, GB 14, STR BR 429 SENT/SERING, SETOR SAO MIGUEL</t>
         </is>
       </c>
     </row>
@@ -1274,46 +1274,46 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>+55 69 993897941</t>
+          <t>+55 69 996096955</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>RUTIELE TAVARES HENKERT - SITIO DA FAMILIA SOARES - BR 429, KM 25, LT 143A, GB 1, STR BR 429 SENT/SERING</t>
+          <t>FELIX SOUZA ESPIRITO SANTO - 1100320055099 - LH 78 SUL, KM 7, LT 60, GB 05, STR BR 429 SENT/SERING || FELIX SOUZA ESPIRITO SANTO - 1100320055099 - LH 78 SUL, KM 7, LT 60, GB 05, STR BR 429 SENT/SERING</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Número inválido</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>+55 69 993904647</t>
+          <t>+55 69 999019031</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>VALDIVIO BONFIM DOS REIS - CH PEDACINHO DO CEU - BR 429, KM 1,5, LT 5B, GB 12, STR BR 429 SENT/ALV</t>
+          <t>VALDECI TIMOTEO - 1100320204476 - LH 90 SUL, KM 7, LT 60-A3, GB 2, STR RO 481</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Enviado</t>
+          <t>Número inválido</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>+55 69 993915285</t>
+          <t>+55 69 999098974</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>KARINA TYEMI CARVALHO - FAZENDA SETE PONTE - LH 22-C-SETE PONTES, KM 5, LT 33,36 E 39, GB TERRA FIRME, STR MANOEL CORREIA, BR 429 KM 155 || KARINA TYEMI CARVALHO - FAZENDA SETE PONTE - LH 22-C-SETE PONTES, KM 5, LT 33,36 E 39, GB TERRA FIRME, STR MANOEL CORREIA, BR 429 KM 155</t>
+          <t>LEONIDAS RAMOS DE SOUZA FILHO - 1100320054597 - LH 94 SUL, KM 12, LT 51 B, GB 1, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -1325,12 +1325,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>+55 69 993949196</t>
+          <t>+55 69 999112125</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>JULIO GUSTAVO PEREIRA DE QUEIROZ - CHACARA BOA ESPERANÇA - ROD. RO 481, KM 2,5, LT 14, GB 4, STR RO 481</t>
+          <t>LUCINEIA DA PENHA BONFANTE - 1100320053536 - LH 94 NORTE, KM 5, LT 20, GB 08, STR RO 481, L.D</t>
         </is>
       </c>
     </row>
@@ -1342,12 +1342,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>+55 69 993966710</t>
+          <t>+55 69 999126066</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>SIDNEY FERREIRA DE SOUZA - FAZENDA BOA ESPERANÇA - LH 74 SUL, KM 48, LT 21, GB RIO BRANCO, STR PRIMAVERA || SIDNEY FERREIRA DE SOUZA - SITIO DOIS IRMAOS - LH 78 SUL, KM 20, LT 146, GB 05, STR BR 429 SENT/SERING</t>
+          <t>FRANCISCO ALVES DA SILVA - 1100320053816 - LH 90 SUL, KM 16, LT 130-B, GB 02, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -1359,29 +1359,29 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>+55 69 996058487</t>
+          <t>+55 69 999143327</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>LUCAS DOMINGOS DIAS - CHACARA SILVA - LH 82 SUL, KM 5, LT 39 A, GB 5, STR RO 481, DESMEMBRADO</t>
+          <t>JOVINO RODRIGUES DA COSTA - 1100320053376 - LH 98 SUL, KM 7, LT 50, GB 10, STR RO 481, DEPOIS DO CAMPO 750 METRO</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Número inválido</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>+55 69 999098974</t>
+          <t>+55 69 999205960</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>LEONIDAS RAMOS DE SOUZA FILHO - SITIO RIO GRANDE - LH 90 SUL, KM 15,5, LT 123, GB 03, STR RO 481, SUL || LEONIDAS RAMOS DE SOUZA FILHO - CH BOA ESPERAÇA - LH 94 SUL, KM 12, LT 51 B, GB 1, STR RO 481</t>
+          <t>JOSMARIO DINIZ DE MATOS - 110032005647 - ROD. RO 481, KM 8, LT 01, GB 10, STR RO 481, DESMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -1393,12 +1393,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>+55 69 999146496</t>
+          <t>+55 69 999229214</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>EDILSON CAVALCANTE PROCOPIO - CHACARA PROCOPIO - LH 94 NORTE, KM 6,5, LT 24 - B1, GB 8, STR RO 481 || EDILSON CAVALCANTE PROCOPIO - CHACARA PROCOPIO - LH 94 NORTE, KM 6,5, LT 24 - B1, GB 8, STR RO 481</t>
+          <t>NARCISO ROSA - 1100320051285 - LH 78 SUL, KM 8, LT 65, GB 6, STR BR 429 SENT/SERING, DESMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -1410,12 +1410,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>+55 69 999191109</t>
+          <t>+55 69 999232663</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>LUCAS DOMINGOS DIAS - CHACARA SILVA - LH 82 SUL, KM 5, LT 39 A, GB 5, STR RO 481, DESMEMBRADO</t>
+          <t>BRUNO FARIAS CRAUSE - 1100320054138 - LH 94 NORTE, KM 4, LT 29, GB 09, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -1427,12 +1427,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>+55 69 999205960</t>
+          <t>+55 69 999242057</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>JOSMARIO DINIZ DE MATOS - SITIO BELA VISTA - ROD. RO 481, KM 8, LT 01, GB 10, STR RO 481, DESMEMBRADO</t>
+          <t>ROGERIA DE OLIVEIRA PINTO - 1100320053898 - LH 86 SUL, KM 20, LT 151, GB 4, STR SANTANA, DESMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -1444,12 +1444,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>+55 69 999222396</t>
+          <t>+55 69 999268048</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>LUIZ FELIPE SILVA - SITIO NORTE SUL - LH 94 SUL, KM 3, LT 14 C, 14D E 14 REMANESCENTE, GB 1, STR RO 481, L.E APOS ASSOCIAÇAO - FUNDIARIA</t>
+          <t>GEISILANDE BRAZ DUARTE - 1100320051809 - LH 90 SUL, KM 2,5, LT 22, GB 02, STR RO 481, DESMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -1461,12 +1461,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>+55 69 999400839</t>
+          <t>+55 69 999340680</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>TCHARLLIS SOUZA BRANDT - SITIO PARAISO - LH 98 SUL, KM 4, LT 76A, GB 10, STR RO 481, DESMEMBRADO</t>
+          <t>GUMERCINO MARTINS GUIMARAES - 1100320053577 - LH 90 NORTE- NOVENTINHA, KM 2, LT 20, GB 09, STR RO 481, DESMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -1478,29 +1478,29 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>+55 69 999404334</t>
+          <t>+55 69 999344380</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>ALEIDA DE OLIVEIRA - nan - LH 94 SUL, KM 13, LT 55, GB 01, STR RO 481, DESMEMBRADA CONFORME ESDRITURA DE PARTILHA</t>
+          <t>FLORIZA ALVES DE OLIVEIRA - 1100320054275 - LH 94 SUL, KM 9, LT 37, GB 1, STR RO 481</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Número inválido</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>+55 69 999462417</t>
+          <t>+55 69 999419677</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>VALDEMAR CLAUDINO DOS SANTOS - SITIO GOIAS - LH 98 NORTE, KM 5, LT 17, GB 16, STR RO 481</t>
+          <t>WALLAFE DO NASCIMENTO CAETANO - 1100320051253 - LH 86 SUL, KM 5, LT 41, GB 04, STR RO 481, DESMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -1512,12 +1512,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>+55 69 999668080</t>
+          <t>+55 69 999455742</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>ADRIELSON CAUTULINO DE SOUZA - SITIO SANTA IZABEL - LH 94 SUL, KM 2,5, LT 10, GB 01, STR RO 481, DESMEMBRADO</t>
+          <t>APARECIDO ANTONIO DE SOUZA - 110032005260 - LH 94 SUL, KM 4, LT 029, GB 002, STR RO 481 || APARECIDO ANTONIO DE SOUZA - 110032005260 - LH 94 SUL, KM 4, LT 029, GB 002, STR RO 481</t>
         </is>
       </c>
     </row>
@@ -1529,12 +1529,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>+55 69 999845726</t>
+          <t>+55 69 999612659</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>VALDETE GONÇALVES - SITIO BOA SORTE - LH 94 NORTE, KM 3, LT 13, GB 08, STR RO 481</t>
+          <t>GEISILANDE BRAZ DUARTE - 1100320051809 - LH 90 SUL, KM 2,5, LT 22, GB 02, STR RO 481, DESMEMBRADO</t>
         </is>
       </c>
     </row>
@@ -1546,12 +1546,46 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>+55 69 999962491</t>
+          <t>+55 69 999621815</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>ALEX JACINTO DE SOUZA - CHACARA D.E.B - ROD. RO 481, KM 10, LT 16-B-1 E 14 REMANECENTE, GB 02, STR RO 481, FUNDIARIA, ACESSO LH 90 APOS PONTE</t>
+          <t>WILSON ROSA DE ALMEIDA - 1100320051655 - BR 429, KM 25, LT 22-F, GB 05, STR BR 429 SENT/ALV, DESMEMBRADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>+55 69 999804992</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>VALDEIR TIMOTEO - 1100320053656 - LH 90 SUL, KM 7, LT 60, GB 2, STR RO 481</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>+55 69 99996857</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>GILMAR BELIZARIO DA SILVA - 1100320054256 - LH 78 SUL, KM 5, LT 35 B, GB 06, STR BR 429 SENT/SERING</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ultima versao com envio pra inadimplentesoutros animais
</commit_message>
<xml_diff>
--- a/BancoProd.xlsx
+++ b/BancoProd.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,12 +458,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>+55 69 36421238</t>
+          <t>+55 69 984096742</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CLAUDIO DA SILVA - SITIO DUAS IRMAS - LH 78 SUL, KM 18, LT 130-A, GB 05, STR BR 429 SENT/SERING || EDIVALDO CARLOS DE OLIVEIRA - ST. FLOR DA MATA - LH 78 SUL, KM 20, LT 144, GB 05, STR BR 429 SENT/SERING || CLAUDIO DA SILVA - SITIO DUAS IRMAS - LH 78 SUL, KM 18, LT 130-A, GB 05, STR BR 429 SENT/SERING || CLAUDIO DA SILVA - SITIO DUAS IRMAS - LH 78 SUL, KM 18, LT 130-A, GB 05, STR BR 429 SENT/SERING</t>
+          <t>LUCIANO KOVALCHUK - LH 78 SUL, KM 1, LT 29C , GB 11, STR BR 429 SENT/SERING - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE || LUCIANO KOVALCHUK - LH 78 SUL, KM 1, LT 29C , GB 11, STR BR 429 SENT/SERING - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
         </is>
       </c>
     </row>
@@ -475,12 +475,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>+55 69 984397155</t>
+          <t>+55 69 984101481</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>LUCIA PEREIRA DOS SANTOS - SITIO TERRA ROXA - ROD. RO 481, KM 17, LT 3, GB RIO BRANCO, STR RO 481, DESMEMBRADO</t>
+          <t>NIRALVA DE OLIVEIRA SILVA - LH 74 SUL, KM 8,5, LT 90, GB 9, STR BR 429 SENT/SERING, DESMEMBRADO - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
         </is>
       </c>
     </row>
@@ -492,12 +492,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>+55 69 984528653</t>
+          <t>+55 69 984396694</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>VANDERLEI DE OLIVEIRA CORDEIRO - SITIO SOLO RICO - LH 86 SUL, KM 20, LT 01B, GB 01, STR RO 481</t>
+          <t>JESSICA VENANCIO DA SILVA - LH 98 NORTE, KM 5,5, LT 19, GB 16, STR RO 481 - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
         </is>
       </c>
     </row>
@@ -509,12 +509,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>+55 69 984753371</t>
+          <t>+55 69 984421186</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CACILDA RIBEIRO ALVES - SITIO ESTRELA DALVA - LH 90 SUL, KM 6, LT 47 -D, GB 03, STR RO 481, DESMEMBRADO</t>
+          <t>CLARICE DE FATIMA SOARES NUNES - BR 429, KM 5, LT 33, GB 11, STR BR 429 SENT/SERING - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
         </is>
       </c>
     </row>
@@ -526,12 +526,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>+55 69 992191613</t>
+          <t>+55 69 984432856</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>HEBERSON DA SILVA JULIO - SITIO DOIS IRMAO - LH 09 SUL, KM 8, LT 56, GB 01, STR BR 429 SENT/SERING</t>
+          <t>MANNEZA JORDANIA BERNARDES DE OLIVEIRA - LH 82 SUL, KM 6, LT 33, GB 5, STR RO 481, DESMEMBRADO - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE || MANNEZA JORDANIA BERNARDES DE OLIVEIRA - LH 82 SUL, KM 6, LT 33, GB 5, STR RO 481, DESMEMBRADO - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
         </is>
       </c>
     </row>
@@ -543,29 +543,29 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>+55 69 992338411</t>
+          <t>+55 69 984735692</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ADAIR DE FREITAS - SITIO BOA ESPERANÇA - LH 25 (MORTA), KM 3, LT 13A, GB 05, STR RO 481</t>
+          <t>LUIS DEOTI - BR 429, KM 2, LT 06, GB 11, STR BR 429 SENT/ALV - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE || LUIS DEOTI - BR 429, KM 2, LT 06, GB 11, STR BR 429 SENT/ALV - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE || LUIS DEOTI - BR 429, KM 2, LT 06, GB 11, STR BR 429 SENT/ALV - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Número inválido</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>+55 69 992390695</t>
+          <t>+55 69 984835481</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CACILDA RIBEIRO ALVES - SITIO ESTRELA DALVA - LH 90 SUL, KM 6, LT 47 -D, GB 03, STR RO 481, DESMEMBRADO</t>
+          <t>SIDNEI BARBOSA SIMAS - LH 25 (MORTA), KM 1,5, LT 05, GB 05, STR BR 429 SENT/SERING - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
         </is>
       </c>
     </row>
@@ -577,12 +577,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>+55 69 992495947</t>
+          <t>+55 69 984956474</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>LUCIANO GOMES RIBEIRO - CHACARA L A - LH 25, KM 8, LT 44, GB 01, STR BR 429 SENT/SERING || LUCIANO GOMES RIBEIRO - CHACARA L A - LH 25, KM 8, LT 44, GB 01, STR BR 429 SENT/SERING || LUCIANO GOMES RIBEIRO - CHACARA L A - LH 25, KM 8, LT 44, GB 01, STR BR 429 SENT/SERING</t>
+          <t>REMY CARDOSO XAVIER - LH 94 NORTE, KM 3,5, LT 25A, GB 9, STR RO 481 - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
         </is>
       </c>
     </row>
@@ -594,12 +594,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>+55 69 992742030</t>
+          <t>+55 69 992035882</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>EDILSON MIRANDA DA SILVA - SITIO BELA VISTA - LH 86 SUL, KM 9, LT 78, GB 03, STR RO 481, L E. FUNDO DA IGREJA ASSEMBLEIA APOS CAMPO.</t>
+          <t>JUCELIO DA SILVA PLASTER - LH 90 SUL, KM 5, LT 39, GB 3, STR RO 481 - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
         </is>
       </c>
     </row>
@@ -611,12 +611,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>+55 69 992888672</t>
+          <t>+55 69 992240030</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>SIDNEY FERREIRA DE SOUZA - SITIO DOIS IRMAOS - LH 78 SUL, KM 20, LT 146, GB 05, STR BR 429 SENT/SERING || SIDNEY FERREIRA DE SOUZA - FAZENDA BOA ESPERANÇA - LH 74 SUL, KM 48, LT 21, GB RIO BRANCO, STR PRIMAVERA</t>
+          <t>MILTON ROSA DE ALMEIDA - BR 429, KM 25, LT 22, STR BR 429 SENT/ALV, DESMENBRADO - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
         </is>
       </c>
     </row>
@@ -628,12 +628,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>+55 69 993161087</t>
+          <t>+55 69 992362662</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>HILTON DE JESUS SOUZA - CHACARA BOM JESUS - LH 78 SUL, KM 12, LT 69, GB 6, STR BR 429 SENT/SERING, DESMEMBRADA</t>
+          <t>VALDOIR LENZ PEREIRA - BR 429, KM 22, LT 99, GB 01, STR BR 429 SENT/SERING - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE || VALDOIR LENZ PEREIRA - BR 429, KM 22, LT 99, GB 01, STR BR 429 SENT/SERING - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
         </is>
       </c>
     </row>
@@ -645,29 +645,29 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>+55 69 993185430</t>
+          <t>+55 69 992526904</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>EILANE GONÇALVES DE ALMEIDA - CHACARA TRES IRMAS - LH 86 SUL, KM 10, LT 86, GB 3, STR RO 481</t>
+          <t>CLERIO MATOS DE ASSIS - LH 78 SUL, KM 3,5, LT 38, GB 11, STR BR 429 SENT/SERING - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Número inválido</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>+55 69 993449821</t>
+          <t>+55 69 992739233</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>EILANE GONÇALVES DE ALMEIDA - CHACARA TRES IRMAS - LH 86 SUL, KM 10, LT 86, GB 3, STR RO 481</t>
+          <t>DANDARA HORANA DE OLIVEIRA GORZA - LH 86 SUL, KM 11, LT 85, GB 04, STR RO 481, L.D - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
         </is>
       </c>
     </row>
@@ -679,12 +679,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>+55 69 993705091</t>
+          <t>+55 69 992759904</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>SILVANA APARECIDA CANHIN SILVA - CHACARA BOM FUTURO - BR 429, KM 2, LT 11-A2, GB 11, STR BR 429 SENT/ALV, L.D FUNDIARIA</t>
+          <t>ANTONIO MARCOS GOMES - BR 429, KM 9,5, LT 22, GB 10, STR BR 429 SENT/SERING, L.D ACESSO IGREJA CRISTA - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
         </is>
       </c>
     </row>
@@ -696,12 +696,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>+55 69 993915285</t>
+          <t>+55 69 992832220</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>KARINA TYEMI CARVALHO - FAZENDA SETE PONTE - LH 22-C-SETE PONTES, KM 5, LT 33,36 E 39, GB TERRA FIRME, STR MANOEL CORREIA, BR 429 KM 155 || KARINA TYEMI CARVALHO - FAZENDA SETE PONTE - LH 22-C-SETE PONTES, KM 5, LT 33,36 E 39, GB TERRA FIRME, STR MANOEL CORREIA, BR 429 KM 155</t>
+          <t>GERALDO GONÇALVES BRANDAO - LH 74 NORTE, KM 4,5, LT 36, GB 14, STR BR 429 SENT/SERING, 2 TRAVESSAO - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
         </is>
       </c>
     </row>
@@ -713,46 +713,420 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>+55 69 993966710</t>
+          <t>+55 69 992836615</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>SIDNEY FERREIRA DE SOUZA - SITIO DOIS IRMAOS - LH 78 SUL, KM 20, LT 146, GB 05, STR BR 429 SENT/SERING || SIDNEY FERREIRA DE SOUZA - FAZENDA BOA ESPERANÇA - LH 74 SUL, KM 48, LT 21, GB RIO BRANCO, STR PRIMAVERA</t>
+          <t>OSMAR FERNANDO BORGES - BR 429, KM 23, LT 263, GB 01, STR BR 429 SENT/SERING - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Número inválido</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>+55 69 999098974</t>
+          <t>+55 69 992946955</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>LEONIDAS RAMOS DE SOUZA FILHO - SITIO RIO GRANDE - LH 90 SUL, KM 15,5, LT 123, GB 03, STR RO 481, SUL || LEONIDAS RAMOS DE SOUZA FILHO - CH BOA ESPERAÇA - LH 94 SUL, KM 12, LT 51 B, GB 1, STR RO 481</t>
+          <t>PEDRO PAULO BOA MORTE VAZ - LH 09 SUL, KM 8, LT 51, GB 001, STR BR 429 SENT/SERING - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Fila de envio</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>+55 69 999845726</t>
+          <t>+55 69 992972422</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>VALDETE GONÇALVES - SITIO BOA SORTE - LH 94 NORTE, KM 3, LT 13, GB 08, STR RO 481</t>
+          <t>DALVACY DA PENHA - BR 429, KM 8, LT 46, GB 11, STR BR 429 SENT/SERING - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>+55 69 993039887</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>GILMAR ANDERSON DA SILVA - LH 98 SUL, KM 12, LT 12, GB 10, STR RO 481, ROD RO 481 - SAO MIGUEL DO GUAPORE - SANTANA DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>+55 69 993139237</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ATAIDE PEREIRA DE SOUZA - LH 82 SUL, KM 6, LT 33, GB 5, STR RO 481, ENFRENTE O TANQUE DE LEITE - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>+55 69 993185430</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>EILANE GONÇALVES DE ALMEIDA - LH 86 SUL, KM 10, LT 86, GB 3, STR RO 481 - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>+55 69 993207066</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>VALDECI TIMOTEO - LH 90 SUL, KM 7, LT 60-A3, GB 2, STR RO 481 - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>+55 69 993266509</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ORLANDINO ALVES DE OLIVEIRA - LH 94 SUL, KM 9, LT 37, GB 1, STR RO 481 - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>+55 69 993277937</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>DANDARA HORANA DE OLIVEIRA GORZA - LH 86 SUL, KM 11, LT 85, GB 04, STR RO 481, L.D - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>+55 69 993317270</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>SIRLENE LIZZI CAVALCANTE - LH 86 SUL, KM 19, LT 149, 149-A, GB 004, STR RO 481 - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>+55 69 993449821</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>EILANE GONÇALVES DE ALMEIDA - LH 86 SUL, KM 10, LT 86, GB 3, STR RO 481 - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>+55 69 993617963</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>ISAIAS STRELOW - LH 98 NORTE, KM 10, LT 34-A, GB 16, STR RO 481, DESMENBRADO - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>+55 69 993780921</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>JUCELIO DA SILVA PLASTER - LH 90 SUL, KM 5, LT 39, GB 3, STR RO 481 - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>+55 69 993860390</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>RAIMUNDO DA CONCEIÇAO SA - BR 429, KM 7,5, LT 20, GB 14, STR BR 429 SENT/SERING, SETOR SAO MIGUEL - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>+55 69 996096955</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>FELIX SOUZA ESPIRITO SANTO - LH 78 SUL, KM 7, LT 60, GB 05, STR BR 429 SENT/SERING - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE || FELIX SOUZA ESPIRITO SANTO - LH 78 SUL, KM 7, LT 60, GB 05, STR BR 429 SENT/SERING - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>+55 69 999019031</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>VALDECI TIMOTEO - LH 90 SUL, KM 7, LT 60-A3, GB 2, STR RO 481 - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>+55 69 999126066</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>FRANCISCO ALVES DA SILVA - LH 90 SUL, KM 16, LT 130-B, GB 02, STR RO 481 - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>+55 69 999232663</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>BRUNO FARIAS CRAUSE - LH 94 NORTE, KM 4, LT 29, GB 09, STR RO 481 - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>+55 69 999268048</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>GEISILANDE BRAZ DUARTE - LH 90 SUL, KM 2,5, LT 22, GB 02, STR RO 481, DESMEMBRADO - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>+55 69 999419677</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>WALLAFE DO NASCIMENTO CAETANO - LH 86 SUL, KM 5, LT 41, GB 04, STR RO 481, DESMEMBRADO - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>+55 69 999455742</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>APARECIDO ANTONIO DE SOUZA - LH 94 SUL, KM 4, LT 029, GB 002, STR RO 481 - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE || APARECIDO ANTONIO DE SOUZA - LH 94 SUL, KM 4, LT 029, GB 002, STR RO 481 - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>+55 69 999612659</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>GEISILANDE BRAZ DUARTE - LH 90 SUL, KM 2,5, LT 22, GB 02, STR RO 481, DESMEMBRADO - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>+55 69 999621815</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>WILSON ROSA DE ALMEIDA - BR 429, KM 25, LT 22-F, GB 05, STR BR 429 SENT/ALV, DESMEMBRADO - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>+55 69 999804992</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>VALDEIR TIMOTEO - LH 90 SUL, KM 7, LT 60, GB 2, STR RO 481 - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>+55 69 99996857</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>GILMAR BELIZARIO DA SILVA - LH 78 SUL, KM 5, LT 35 B, GB 06, STR BR 429 SENT/SERING - SAO MIGUEL DO GUAPORE - SAO MIGUEL DO GUAPORE</t>
         </is>
       </c>
     </row>

</xml_diff>